<commit_message>
login & TestNG,POM update 25-01-20
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -3,27 +3,27 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\eclipse workspace\TestAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="575" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="575" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Login" sheetId="10" r:id="rId1"/>
+    <sheet name="Login" sheetId="12" r:id="rId1"/>
     <sheet name="Lead Entry" sheetId="1" r:id="rId2"/>
     <sheet name="DATA" sheetId="4" state="hidden" r:id="rId3"/>
     <sheet name="Employee" sheetId="5" r:id="rId4"/>
     <sheet name="Batch" sheetId="6" r:id="rId5"/>
     <sheet name="Master" sheetId="7" r:id="rId6"/>
     <sheet name="Lead Assign Details" sheetId="8" r:id="rId7"/>
-    <sheet name="Logs" sheetId="11" r:id="rId8"/>
+    <sheet name="Logs" sheetId="14" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1520" uniqueCount="850">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1524" uniqueCount="851">
   <si>
     <t xml:space="preserve">Input </t>
   </si>
@@ -2571,9 +2571,6 @@
     <t>gjgdfudfyu</t>
   </si>
   <si>
-    <t>fgsdfgudfu</t>
-  </si>
-  <si>
     <t>anand@learnetex.com</t>
   </si>
   <si>
@@ -2595,31 +2592,38 @@
     <t>B.H:anand</t>
   </si>
   <si>
+    <t>ExpectedResult</t>
+  </si>
+  <si>
+    <t>ActualResult</t>
+  </si>
+  <si>
+    <t>Enter User Mail-ID &amp; Password</t>
+  </si>
+  <si>
+    <t>Login Failed. Wrong Username or Password!</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>ExpectedResult</t>
-  </si>
-  <si>
-    <t>ActualResult</t>
-  </si>
-  <si>
-    <t>Enter User Mail-ID &amp; Password</t>
-  </si>
-  <si>
-    <t>Login Failed. Wrong Username or Password!</t>
-  </si>
-  <si>
-    <t>Failed</t>
+    <t>jsdhfjsdfj</t>
+  </si>
+  <si>
+    <t>ghsdfdjkhf</t>
+  </si>
+  <si>
+    <t>Pass123456</t>
+  </si>
+  <si>
+    <t>Passed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2781,7 +2785,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
@@ -2827,6 +2831,7 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3108,89 +3113,98 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B8"/>
+      <selection activeCell="A3" sqref="A3:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="44.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" s="24" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
+        <v>840</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="26" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>834</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>834</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>839</v>
-      </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="1" t="s">
+        <v>848</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>836</v>
+        <v>838</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>838</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>843</v>
-      </c>
-      <c r="B6" t="s">
-        <v>843</v>
+        <v>835</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>849</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
+        <v>846</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>837</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>848</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A8" r:id="rId1"/>
-    <hyperlink ref="A5" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="B4" r:id="rId4" display="http://invalid.uri/"/>
+    <hyperlink ref="A9" r:id="rId1"/>
+    <hyperlink ref="A6" r:id="rId2"/>
+    <hyperlink ref="A5" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -3205,44 +3219,44 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.140625" style="1" collapsed="1"/>
-    <col min="5" max="5" width="10.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.140625" style="1" collapsed="1"/>
-    <col min="8" max="8" width="17.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.140625" style="1" collapsed="1"/>
-    <col min="10" max="10" width="10.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.140625" style="1" collapsed="1"/>
-    <col min="12" max="12" width="12.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="19.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="11.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="21.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="10.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="16.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="20.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="7.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="20.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="15.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="10.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="12.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="28" style="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="16.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="23.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="9.140625" style="1" collapsed="1"/>
-    <col min="29" max="29" width="12.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="9.140625" style="1" collapsed="1"/>
-    <col min="32" max="32" width="11" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="15.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="20.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="15.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="18" style="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="32.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="16.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="17.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="12.7109375" collapsed="true"/>
+    <col min="4" max="4" style="1" width="9.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="10.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="17.5703125" collapsed="true"/>
+    <col min="7" max="7" style="1" width="9.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="17.5703125" collapsed="true"/>
+    <col min="9" max="9" style="1" width="9.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="10.7109375" collapsed="true"/>
+    <col min="11" max="11" style="1" width="9.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="1" width="12.140625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="1" width="11.140625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="1" width="19.5703125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="1" width="21.5703125" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="1" width="10.28515625" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" style="1" width="16.28515625" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="1" width="20.28515625" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="1" width="7.5703125" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" style="1" width="20.28515625" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="1" width="15.5703125" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" style="1" width="10.85546875" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" style="1" width="28.0" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" style="1" width="16.140625" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" style="1" width="23.5703125" collapsed="true"/>
+    <col min="28" max="28" style="1" width="9.140625" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" style="1" width="12.42578125" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" style="1" width="18.7109375" collapsed="true"/>
+    <col min="31" max="31" style="1" width="9.140625" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="11.0" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" style="1" width="15.42578125" collapsed="true"/>
+    <col min="34" max="34" customWidth="true" style="1" width="20.5703125" collapsed="true"/>
+    <col min="35" max="35" customWidth="true" style="1" width="15.42578125" collapsed="true"/>
+    <col min="36" max="36" customWidth="true" style="1" width="18.0" collapsed="true"/>
+    <col min="37" max="37" customWidth="true" style="1" width="32.28515625" collapsed="true"/>
+    <col min="38" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="30" x14ac:dyDescent="0.25">
@@ -4497,14 +4511,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.7109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="25.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="28.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="30.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="25.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="30.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -5267,33 +5281,33 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S15"/>
+  <dimension ref="A1:R15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="30.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="15.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="13" style="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="17.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="14.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="14.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="6.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="21.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="12.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="10.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="12.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="9.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="30.140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="10.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="12.85546875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="1" width="15.42578125" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="1" width="13.0" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="1" width="17.7109375" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="1" width="14.85546875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="1" width="14.140625" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="20" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -6132,147 +6146,147 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="6.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="13" width="7.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="16" width="8.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="11.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="10.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="13" style="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="21" width="9.140625" style="1" collapsed="1"/>
-    <col min="22" max="22" width="11" style="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="9.140625" style="1" collapsed="1"/>
-    <col min="24" max="24" width="11.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="10.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="13" style="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="28" width="9.140625" style="1" collapsed="1"/>
-    <col min="29" max="29" width="11" style="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="9.140625" style="1" collapsed="1"/>
-    <col min="31" max="31" width="11.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="10.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="13" style="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="35" width="9.140625" style="1" collapsed="1"/>
-    <col min="36" max="36" width="11" style="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="9.140625" style="1" collapsed="1"/>
-    <col min="38" max="38" width="11.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="10.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="13" style="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="42" width="9.140625" style="1" collapsed="1"/>
-    <col min="43" max="43" width="11" style="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="9.140625" style="1" collapsed="1"/>
-    <col min="45" max="45" width="11.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="10.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="13" style="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="49" width="9.140625" style="1" collapsed="1"/>
-    <col min="50" max="50" width="11" style="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="9.140625" style="1" collapsed="1"/>
-    <col min="52" max="52" width="11.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="10.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="13" style="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="56" width="9.140625" style="1" collapsed="1"/>
-    <col min="57" max="57" width="11" style="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="9.140625" style="1" collapsed="1"/>
-    <col min="59" max="59" width="11.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="10.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="13" style="1" customWidth="1" collapsed="1"/>
-    <col min="62" max="63" width="9.140625" style="1" collapsed="1"/>
-    <col min="64" max="64" width="11" style="1" customWidth="1" collapsed="1"/>
-    <col min="65" max="65" width="9.140625" style="1" collapsed="1"/>
-    <col min="66" max="66" width="11.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="67" max="67" width="10.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="68" max="68" width="13" style="1" customWidth="1" collapsed="1"/>
-    <col min="69" max="70" width="9.140625" style="1" collapsed="1"/>
-    <col min="71" max="71" width="11" style="1" customWidth="1" collapsed="1"/>
-    <col min="72" max="72" width="9.140625" style="1" collapsed="1"/>
-    <col min="73" max="73" width="11.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="74" max="74" width="10.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="75" max="75" width="13" style="1" customWidth="1" collapsed="1"/>
-    <col min="76" max="77" width="9.140625" style="1" collapsed="1"/>
-    <col min="78" max="78" width="11" style="1" customWidth="1" collapsed="1"/>
-    <col min="79" max="79" width="9.140625" style="1" collapsed="1"/>
-    <col min="80" max="80" width="10.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="81" max="86" width="9.140625" style="1" collapsed="1"/>
-    <col min="87" max="87" width="11.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="88" max="88" width="10.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="89" max="89" width="13" style="1" customWidth="1" collapsed="1"/>
-    <col min="90" max="91" width="9.140625" style="1" collapsed="1"/>
-    <col min="92" max="92" width="11" style="1" customWidth="1" collapsed="1"/>
-    <col min="93" max="93" width="9.140625" style="1" collapsed="1"/>
-    <col min="94" max="94" width="11.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="95" max="95" width="10.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="96" max="96" width="13" style="1" customWidth="1" collapsed="1"/>
-    <col min="97" max="98" width="9.140625" style="1" collapsed="1"/>
-    <col min="99" max="99" width="11" style="1" customWidth="1" collapsed="1"/>
-    <col min="100" max="100" width="9.140625" style="1" collapsed="1"/>
-    <col min="101" max="101" width="11.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="102" max="102" width="10.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="103" max="103" width="13" style="1" customWidth="1" collapsed="1"/>
-    <col min="104" max="105" width="9.140625" style="1" collapsed="1"/>
-    <col min="106" max="106" width="11" style="1" customWidth="1" collapsed="1"/>
-    <col min="107" max="107" width="9.140625" style="1" collapsed="1"/>
-    <col min="108" max="108" width="11.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="109" max="109" width="10.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="110" max="110" width="13" style="1" customWidth="1" collapsed="1"/>
-    <col min="111" max="112" width="9.140625" style="1" collapsed="1"/>
-    <col min="113" max="113" width="11" style="1" customWidth="1" collapsed="1"/>
-    <col min="114" max="114" width="9.140625" style="1" collapsed="1"/>
-    <col min="115" max="115" width="11.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="116" max="116" width="10.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="117" max="117" width="13" style="1" customWidth="1" collapsed="1"/>
-    <col min="118" max="119" width="9.140625" style="1" collapsed="1"/>
-    <col min="120" max="120" width="11" style="1" customWidth="1" collapsed="1"/>
-    <col min="121" max="121" width="9.140625" style="1" collapsed="1"/>
-    <col min="122" max="122" width="11.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="123" max="123" width="10.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="124" max="124" width="13" style="1" customWidth="1" collapsed="1"/>
-    <col min="125" max="126" width="9.140625" style="1" collapsed="1"/>
-    <col min="127" max="127" width="11" style="1" customWidth="1" collapsed="1"/>
-    <col min="128" max="128" width="9.140625" style="1" collapsed="1"/>
-    <col min="129" max="129" width="10.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="130" max="135" width="9.140625" style="1" collapsed="1"/>
-    <col min="136" max="136" width="10.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="137" max="142" width="9.140625" style="1" collapsed="1"/>
-    <col min="143" max="143" width="10.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="144" max="149" width="9.140625" style="1" collapsed="1"/>
-    <col min="150" max="150" width="10.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="151" max="156" width="9.140625" style="1" collapsed="1"/>
-    <col min="157" max="157" width="10.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="158" max="163" width="9.140625" style="1" collapsed="1"/>
-    <col min="164" max="164" width="10.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="165" max="168" width="9.140625" style="1" collapsed="1"/>
-    <col min="169" max="169" width="10.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="170" max="170" width="10.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="171" max="171" width="10.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="172" max="177" width="9.140625" style="1" collapsed="1"/>
-    <col min="178" max="178" width="10.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="179" max="184" width="9.140625" style="1" collapsed="1"/>
-    <col min="185" max="185" width="10.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="186" max="191" width="9.140625" style="1" collapsed="1"/>
-    <col min="192" max="192" width="10.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="193" max="198" width="9.140625" style="1" collapsed="1"/>
-    <col min="199" max="199" width="10.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="200" max="205" width="9.140625" style="1" collapsed="1"/>
-    <col min="206" max="206" width="10.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="207" max="212" width="9.140625" style="1" collapsed="1"/>
-    <col min="213" max="213" width="10.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="214" max="219" width="9.140625" style="1" collapsed="1"/>
-    <col min="220" max="220" width="10.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="221" max="221" width="12.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="222" max="222" width="12" style="1" customWidth="1" collapsed="1"/>
-    <col min="223" max="223" width="12.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="224" max="224" width="13" style="1" customWidth="1" collapsed="1"/>
-    <col min="225" max="225" width="12" style="1" customWidth="1" collapsed="1"/>
-    <col min="226" max="226" width="11.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="227" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="11.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="15.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="16.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="14.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="18.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="14.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="14.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="17.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="1" width="6.7109375" collapsed="true"/>
+    <col min="12" max="13" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="14" max="16" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" style="1" width="10.28515625" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="1" width="13.0" collapsed="true"/>
+    <col min="20" max="21" style="1" width="9.140625" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="1" width="11.0" collapsed="true"/>
+    <col min="23" max="23" style="1" width="9.140625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" style="1" width="10.28515625" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" style="1" width="13.0" collapsed="true"/>
+    <col min="27" max="28" style="1" width="9.140625" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" style="1" width="11.0" collapsed="true"/>
+    <col min="30" max="30" style="1" width="9.140625" collapsed="true"/>
+    <col min="31" max="31" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="32" max="32" customWidth="true" style="1" width="10.28515625" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" style="1" width="13.0" collapsed="true"/>
+    <col min="34" max="35" style="1" width="9.140625" collapsed="true"/>
+    <col min="36" max="36" customWidth="true" style="1" width="11.0" collapsed="true"/>
+    <col min="37" max="37" style="1" width="9.140625" collapsed="true"/>
+    <col min="38" max="38" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="39" max="39" customWidth="true" style="1" width="10.28515625" collapsed="true"/>
+    <col min="40" max="40" customWidth="true" style="1" width="13.0" collapsed="true"/>
+    <col min="41" max="42" style="1" width="9.140625" collapsed="true"/>
+    <col min="43" max="43" customWidth="true" style="1" width="11.0" collapsed="true"/>
+    <col min="44" max="44" style="1" width="9.140625" collapsed="true"/>
+    <col min="45" max="45" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="46" max="46" customWidth="true" style="1" width="10.28515625" collapsed="true"/>
+    <col min="47" max="47" customWidth="true" style="1" width="13.0" collapsed="true"/>
+    <col min="48" max="49" style="1" width="9.140625" collapsed="true"/>
+    <col min="50" max="50" customWidth="true" style="1" width="11.0" collapsed="true"/>
+    <col min="51" max="51" style="1" width="9.140625" collapsed="true"/>
+    <col min="52" max="52" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="53" max="53" customWidth="true" style="1" width="10.28515625" collapsed="true"/>
+    <col min="54" max="54" customWidth="true" style="1" width="13.0" collapsed="true"/>
+    <col min="55" max="56" style="1" width="9.140625" collapsed="true"/>
+    <col min="57" max="57" customWidth="true" style="1" width="11.0" collapsed="true"/>
+    <col min="58" max="58" style="1" width="9.140625" collapsed="true"/>
+    <col min="59" max="59" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="60" max="60" customWidth="true" style="1" width="10.28515625" collapsed="true"/>
+    <col min="61" max="61" customWidth="true" style="1" width="13.0" collapsed="true"/>
+    <col min="62" max="63" style="1" width="9.140625" collapsed="true"/>
+    <col min="64" max="64" customWidth="true" style="1" width="11.0" collapsed="true"/>
+    <col min="65" max="65" style="1" width="9.140625" collapsed="true"/>
+    <col min="66" max="66" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="67" max="67" customWidth="true" style="1" width="10.28515625" collapsed="true"/>
+    <col min="68" max="68" customWidth="true" style="1" width="13.0" collapsed="true"/>
+    <col min="69" max="70" style="1" width="9.140625" collapsed="true"/>
+    <col min="71" max="71" customWidth="true" style="1" width="11.0" collapsed="true"/>
+    <col min="72" max="72" style="1" width="9.140625" collapsed="true"/>
+    <col min="73" max="73" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="74" max="74" customWidth="true" style="1" width="10.28515625" collapsed="true"/>
+    <col min="75" max="75" customWidth="true" style="1" width="13.0" collapsed="true"/>
+    <col min="76" max="77" style="1" width="9.140625" collapsed="true"/>
+    <col min="78" max="78" customWidth="true" style="1" width="11.0" collapsed="true"/>
+    <col min="79" max="79" style="1" width="9.140625" collapsed="true"/>
+    <col min="80" max="80" bestFit="true" customWidth="true" style="1" width="10.42578125" collapsed="true"/>
+    <col min="81" max="86" style="1" width="9.140625" collapsed="true"/>
+    <col min="87" max="87" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="88" max="88" customWidth="true" style="1" width="10.28515625" collapsed="true"/>
+    <col min="89" max="89" customWidth="true" style="1" width="13.0" collapsed="true"/>
+    <col min="90" max="91" style="1" width="9.140625" collapsed="true"/>
+    <col min="92" max="92" customWidth="true" style="1" width="11.0" collapsed="true"/>
+    <col min="93" max="93" style="1" width="9.140625" collapsed="true"/>
+    <col min="94" max="94" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="95" max="95" customWidth="true" style="1" width="10.28515625" collapsed="true"/>
+    <col min="96" max="96" customWidth="true" style="1" width="13.0" collapsed="true"/>
+    <col min="97" max="98" style="1" width="9.140625" collapsed="true"/>
+    <col min="99" max="99" customWidth="true" style="1" width="11.0" collapsed="true"/>
+    <col min="100" max="100" style="1" width="9.140625" collapsed="true"/>
+    <col min="101" max="101" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="102" max="102" customWidth="true" style="1" width="10.28515625" collapsed="true"/>
+    <col min="103" max="103" customWidth="true" style="1" width="13.0" collapsed="true"/>
+    <col min="104" max="105" style="1" width="9.140625" collapsed="true"/>
+    <col min="106" max="106" customWidth="true" style="1" width="11.0" collapsed="true"/>
+    <col min="107" max="107" style="1" width="9.140625" collapsed="true"/>
+    <col min="108" max="108" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="109" max="109" customWidth="true" style="1" width="10.28515625" collapsed="true"/>
+    <col min="110" max="110" customWidth="true" style="1" width="13.0" collapsed="true"/>
+    <col min="111" max="112" style="1" width="9.140625" collapsed="true"/>
+    <col min="113" max="113" customWidth="true" style="1" width="11.0" collapsed="true"/>
+    <col min="114" max="114" style="1" width="9.140625" collapsed="true"/>
+    <col min="115" max="115" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="116" max="116" customWidth="true" style="1" width="10.28515625" collapsed="true"/>
+    <col min="117" max="117" customWidth="true" style="1" width="13.0" collapsed="true"/>
+    <col min="118" max="119" style="1" width="9.140625" collapsed="true"/>
+    <col min="120" max="120" customWidth="true" style="1" width="11.0" collapsed="true"/>
+    <col min="121" max="121" style="1" width="9.140625" collapsed="true"/>
+    <col min="122" max="122" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="123" max="123" customWidth="true" style="1" width="10.28515625" collapsed="true"/>
+    <col min="124" max="124" customWidth="true" style="1" width="13.0" collapsed="true"/>
+    <col min="125" max="126" style="1" width="9.140625" collapsed="true"/>
+    <col min="127" max="127" customWidth="true" style="1" width="11.0" collapsed="true"/>
+    <col min="128" max="128" style="1" width="9.140625" collapsed="true"/>
+    <col min="129" max="129" bestFit="true" customWidth="true" style="1" width="10.42578125" collapsed="true"/>
+    <col min="130" max="135" style="1" width="9.140625" collapsed="true"/>
+    <col min="136" max="136" bestFit="true" customWidth="true" style="1" width="10.42578125" collapsed="true"/>
+    <col min="137" max="142" style="1" width="9.140625" collapsed="true"/>
+    <col min="143" max="143" bestFit="true" customWidth="true" style="1" width="10.42578125" collapsed="true"/>
+    <col min="144" max="149" style="1" width="9.140625" collapsed="true"/>
+    <col min="150" max="150" bestFit="true" customWidth="true" style="1" width="10.42578125" collapsed="true"/>
+    <col min="151" max="156" style="1" width="9.140625" collapsed="true"/>
+    <col min="157" max="157" bestFit="true" customWidth="true" style="1" width="10.7109375" collapsed="true"/>
+    <col min="158" max="163" style="1" width="9.140625" collapsed="true"/>
+    <col min="164" max="164" bestFit="true" customWidth="true" style="1" width="10.42578125" collapsed="true"/>
+    <col min="165" max="168" style="1" width="9.140625" collapsed="true"/>
+    <col min="169" max="169" customWidth="true" style="1" width="10.7109375" collapsed="true"/>
+    <col min="170" max="170" customWidth="true" style="1" width="10.42578125" collapsed="true"/>
+    <col min="171" max="171" bestFit="true" customWidth="true" style="1" width="10.42578125" collapsed="true"/>
+    <col min="172" max="177" style="1" width="9.140625" collapsed="true"/>
+    <col min="178" max="178" bestFit="true" customWidth="true" style="1" width="10.42578125" collapsed="true"/>
+    <col min="179" max="184" style="1" width="9.140625" collapsed="true"/>
+    <col min="185" max="185" bestFit="true" customWidth="true" style="1" width="10.42578125" collapsed="true"/>
+    <col min="186" max="191" style="1" width="9.140625" collapsed="true"/>
+    <col min="192" max="192" bestFit="true" customWidth="true" style="1" width="10.7109375" collapsed="true"/>
+    <col min="193" max="198" style="1" width="9.140625" collapsed="true"/>
+    <col min="199" max="199" bestFit="true" customWidth="true" style="1" width="10.7109375" collapsed="true"/>
+    <col min="200" max="205" style="1" width="9.140625" collapsed="true"/>
+    <col min="206" max="206" bestFit="true" customWidth="true" style="1" width="10.7109375" collapsed="true"/>
+    <col min="207" max="212" style="1" width="9.140625" collapsed="true"/>
+    <col min="213" max="213" bestFit="true" customWidth="true" style="1" width="10.42578125" collapsed="true"/>
+    <col min="214" max="219" style="1" width="9.140625" collapsed="true"/>
+    <col min="220" max="220" bestFit="true" customWidth="true" style="1" width="10.42578125" collapsed="true"/>
+    <col min="221" max="221" customWidth="true" style="1" width="12.7109375" collapsed="true"/>
+    <col min="222" max="222" customWidth="true" style="1" width="12.0" collapsed="true"/>
+    <col min="223" max="223" customWidth="true" style="1" width="12.140625" collapsed="true"/>
+    <col min="224" max="224" customWidth="true" style="1" width="13.0" collapsed="true"/>
+    <col min="225" max="225" customWidth="true" style="1" width="12.0" collapsed="true"/>
+    <col min="226" max="226" customWidth="true" style="1" width="11.5703125" collapsed="true"/>
+    <col min="227" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:297" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -8138,9 +8152,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -8213,16 +8227,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" style="16" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="26.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="16" width="13.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="26.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="13.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -8605,25 +8619,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="43.28515625" customWidth="1"/>
-    <col min="4" max="4" width="41.140625" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="29.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="41.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="31.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="23.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="24" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="25" t="s">
+      <c r="A1" s="29" t="s">
+        <v>840</v>
+      </c>
+      <c r="B1" s="24" t="s">
         <v>841</v>
-      </c>
-      <c r="C1" s="24" t="s">
-        <v>842</v>
       </c>
       <c r="D1" s="25"/>
     </row>
@@ -8635,13 +8649,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="E2" s="27" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -8649,13 +8663,13 @@
         <v>834</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>835</v>
+        <v>847</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="E3" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -8663,66 +8677,58 @@
         <v>143</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1</v>
+        <v>848</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="E4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="E5" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>2</v>
+        <v>849</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>848</v>
-      </c>
-      <c r="E6" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="A7" s="2" t="s">
+        <v>846</v>
+      </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>847</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" t="s">
         <v>844</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>837</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>838</v>
-      </c>
       <c r="C8" s="28" t="s">
-        <v>848</v>
-      </c>
-      <c r="E8" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -8743,6 +8749,5 @@
     <hyperlink ref="B5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>